<commit_message>
Korrekturen in GD und annotations
</commit_message>
<xml_diff>
--- a/data/variables/ds1/variables.xlsx
+++ b/data/variables/ds1/variables.xlsx
@@ -2651,13 +2651,7 @@
     <t>Diese Variable wurde zum Zweck der Anonymisierung durch Aggregation aus der Staatsangehörigkeitsvariable (bei Ausland) generiert. Zur Aggregation wurde eine projekteigene Codierliste (in Anlehnung an die Länderklassifikation des NEPS bei der Startkohorte 5, aber mit Anpassungen bei den europäischen Ländern) verwendet (vgl. cl-dzhw-23). Zu Einzelheiten vgl. Generierungsregel.</t>
   </si>
   <si>
-    <t>Diese Variable wurde zum Zweck der Anonymisierung durch Aggregation aus der Staatsangehörigkeitsvariable (bei Ausland) generiert. Zur Aggregation wurde eine projekteigene Codierliste verwendet (vgl. cl-dzhw-23). Dabei wurde die Türkei wurde zu Asien und Russland zu Europa außerhalb der EU codiert. Zu Einzelheiten vgl. Generierungsregel.</t>
-  </si>
-  <si>
     <t>Diese Variable wurde zum Zweck der Anonymisierung durch Aggregation aus der Geburtslandvariable (bei Ausland) generiert. Zur Aggregation wurde eine projekteigene Codierliste (in Anlehnung an die Länderklassifikation des NEPS bei der Startkohorte 5, aber mit Anpassungen bei den europäischen Ländern) verwendet (vgl. cl-dzhw-23). Zu Einzelheiten vgl. Generierungsregel.</t>
-  </si>
-  <si>
-    <t>Diese Variable wurde zum Zweck der Anonymisierung durch Aggregation aus der Geburtslandvariable (bei Ausland) generiert. Zur Aggregation wurde eine projekteigene Codierliste verwendet (vgl. cl-dzhw-23). Dabei wurde die Türkei wurde zu Asien und Russland zu Europa außerhalb der EU codiert. Zu Einzelheiten vgl. Generierungsregel.</t>
   </si>
   <si>
     <t>Diese Variable wurde zum Zweck der Anonymisierung aus der Wohnsitzvariable (erfasst als dreistellige Postleitzahl) generiert. Zur Aggregation wurde die Referenzliste "Tercet NUTS-postal codes matching tables" des Statistischen Amtes der Europäischen Union (Eurostat) von 2010 verwendet (cl-eurostat-deplznuts-2010). Diese Referenzliste weist die fünfstellige Postleitzahl und die zugehörige NUTS-3 Region aus. Daraus wurden die dreistelligen Postleitzahlen und die NUTS-2 Regionen gebildet. Sofern die dreistellige Postleitzahl nicht eindeutig einer NUTS-2-Region zugeordnet werden konnte, wurde der Missingwert "-966 nicht bestimmbar" vergeben.</t>
@@ -2843,78 +2837,6 @@
     <t>generationDetails.ruleExpressionLanguage</t>
   </si>
   <si>
-    <t>gra2009-ds1-dem08b_g1o</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem08b_g2r</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem08b_g3d</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-sys01a_o</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-sys01b_o</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-sys01c_o</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ04a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ04b</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ10</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ262</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ342a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ342b</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ342c</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ352</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ37a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-occ37b</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem08a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem151a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem151b</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem152a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem152b</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem153a</t>
-  </si>
-  <si>
-    <t>gra2009-ds1-dem153b</t>
-  </si>
-  <si>
-    <t>recode adem07_d (1942/1959 = 1), gen (adem07_g1)</t>
-  </si>
-  <si>
     <t>recode aocc242j_g2d (1/10 92 =1) (11/16 91 = 2), gen(aocc242j_g3)</t>
   </si>
   <si>
@@ -2941,6 +2863,84 @@
   </si>
   <si>
     <t>Haben die Befragten mehr als drei Kinder angegeben, wurden die Geburtsdaten des ältesten und des jüngsten Kindes beibehalten. Angaben zu den mittleren Kindern wurden gestrichen und durch die Angaben zum jüngsten bzw. ältesten Kind ersetzt.</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ04a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ04b_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ10_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ262_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ342a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ342b_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ342c_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ352_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ37a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-occ37b_c</t>
+  </si>
+  <si>
+    <t>recode adem07_d (1942/1959 = 1), gen(adem07_g1)</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem08a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem08b_g1o</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem08b_g2r</t>
+  </si>
+  <si>
+    <t>Diese Variable wurde zum Zweck der Anonymisierung durch Aggregation aus der Staatsangehörigkeitsvariable (bei Ausland) generiert. Zur Aggregation wurde eine projekteigene Codierliste verwendet (vgl. cl-dzhw-23). Dabei wurde die Türkei zu Asien und Russland zu Europa außerhalb der EU codiert. Zu Einzelheiten vgl. Generierungsregel.</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem08b_g3d</t>
+  </si>
+  <si>
+    <t>Diese Variable wurde zum Zweck der Anonymisierung durch Aggregation aus der Geburtslandvariable (bei Ausland) generiert. Zur Aggregation wurde eine projekteigene Codierliste verwendet (vgl. cl-dzhw-23). Dabei wurde die Türkei zu Asien und Russland zu Europa außerhalb der EU codiert. Zu Einzelheiten vgl. Generierungsregel.</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem151a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem151b_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem152a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem152b_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem153a_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-dem153b_c</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-sys01a_o</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-sys01b_o</t>
+  </si>
+  <si>
+    <t>abs2009-ds1-sys01c_o</t>
   </si>
 </sst>
 </file>
@@ -2973,11 +2973,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3281,57 +3278,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N811"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A775" workbookViewId="0">
-      <selection activeCell="B794" sqref="B794"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D1" t="s">
         <v>814</v>
       </c>
       <c r="E1" t="s">
+        <v>926</v>
+      </c>
+      <c r="F1" t="s">
+        <v>927</v>
+      </c>
+      <c r="G1" t="s">
         <v>928</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>929</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>930</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>931</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>932</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>933</v>
       </c>
-      <c r="K1" t="s">
-        <v>934</v>
-      </c>
-      <c r="L1" t="s">
-        <v>935</v>
-      </c>
       <c r="M1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="N1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -3934,7 +3928,7 @@
         <v>840</v>
       </c>
       <c r="K22" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="L22" t="s">
         <v>832</v>
@@ -3992,7 +3986,7 @@
         <v>842</v>
       </c>
       <c r="K24" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="L24" t="s">
         <v>832</v>
@@ -4572,7 +4566,7 @@
         <v>840</v>
       </c>
       <c r="K44" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="L44" t="s">
         <v>832</v>
@@ -4630,7 +4624,7 @@
         <v>842</v>
       </c>
       <c r="K46" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="L46" t="s">
         <v>832</v>
@@ -5210,7 +5204,7 @@
         <v>840</v>
       </c>
       <c r="K66" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="L66" t="s">
         <v>832</v>
@@ -5268,7 +5262,7 @@
         <v>842</v>
       </c>
       <c r="K68" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="L68" t="s">
         <v>832</v>
@@ -5848,7 +5842,7 @@
         <v>840</v>
       </c>
       <c r="K88" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="L88" t="s">
         <v>832</v>
@@ -5906,7 +5900,7 @@
         <v>842</v>
       </c>
       <c r="K90" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L90" t="s">
         <v>832</v>
@@ -6486,7 +6480,7 @@
         <v>840</v>
       </c>
       <c r="K110" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="L110" t="s">
         <v>832</v>
@@ -6544,7 +6538,7 @@
         <v>842</v>
       </c>
       <c r="K112" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="L112" t="s">
         <v>832</v>
@@ -7008,7 +7002,7 @@
         <v>840</v>
       </c>
       <c r="K128" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="L128" t="s">
         <v>832</v>
@@ -7066,7 +7060,7 @@
         <v>842</v>
       </c>
       <c r="K130" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="L130" t="s">
         <v>832</v>
@@ -7530,7 +7524,7 @@
         <v>840</v>
       </c>
       <c r="K146" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="L146" t="s">
         <v>832</v>
@@ -7588,7 +7582,7 @@
         <v>842</v>
       </c>
       <c r="K148" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="L148" t="s">
         <v>832</v>
@@ -8052,7 +8046,7 @@
         <v>840</v>
       </c>
       <c r="K164" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="L164" t="s">
         <v>832</v>
@@ -8110,7 +8104,7 @@
         <v>842</v>
       </c>
       <c r="K166" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="L166" t="s">
         <v>832</v>
@@ -13243,7 +13237,7 @@
         <v>840</v>
       </c>
       <c r="K343" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="L343" t="s">
         <v>832</v>
@@ -13301,7 +13295,7 @@
         <v>842</v>
       </c>
       <c r="K345" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="L345" t="s">
         <v>832</v>
@@ -13417,7 +13411,7 @@
         <v>840</v>
       </c>
       <c r="K349" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="L349" t="s">
         <v>832</v>
@@ -13475,7 +13469,7 @@
         <v>842</v>
       </c>
       <c r="K351" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="L351" t="s">
         <v>832</v>
@@ -13591,7 +13585,7 @@
         <v>840</v>
       </c>
       <c r="K355" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="L355" t="s">
         <v>832</v>
@@ -13649,7 +13643,7 @@
         <v>842</v>
       </c>
       <c r="K357" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="L357" t="s">
         <v>832</v>
@@ -14258,7 +14252,7 @@
         <v>840</v>
       </c>
       <c r="K378" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="L378" t="s">
         <v>832</v>
@@ -14316,7 +14310,7 @@
         <v>842</v>
       </c>
       <c r="K380" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="L380" t="s">
         <v>832</v>
@@ -14432,7 +14426,7 @@
         <v>840</v>
       </c>
       <c r="K384" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="L384" t="s">
         <v>832</v>
@@ -14490,7 +14484,7 @@
         <v>842</v>
       </c>
       <c r="K386" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="L386" t="s">
         <v>832</v>
@@ -14606,7 +14600,7 @@
         <v>840</v>
       </c>
       <c r="K390" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="L390" t="s">
         <v>832</v>
@@ -14664,7 +14658,7 @@
         <v>842</v>
       </c>
       <c r="K392" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="L392" t="s">
         <v>832</v>
@@ -15975,7 +15969,7 @@
         <v>811</v>
       </c>
       <c r="M437" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="438" spans="1:13" x14ac:dyDescent="0.2">
@@ -16004,7 +15998,7 @@
         <v>811</v>
       </c>
       <c r="M438" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="439" spans="1:13" x14ac:dyDescent="0.2">
@@ -16613,15 +16607,15 @@
         <v>811</v>
       </c>
       <c r="M459" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="460" spans="1:13" ht="409.5" x14ac:dyDescent="0.2">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="460" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>459</v>
       </c>
-      <c r="B460" s="1" t="s">
-        <v>965</v>
+      <c r="B460" t="s">
+        <v>939</v>
       </c>
       <c r="D460" t="s">
         <v>815</v>
@@ -18666,7 +18660,7 @@
         <v>855</v>
       </c>
       <c r="K530" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="L530" t="s">
         <v>832</v>
@@ -18695,7 +18689,7 @@
         <v>856</v>
       </c>
       <c r="K531" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="L531" t="s">
         <v>832</v>
@@ -19072,7 +19066,7 @@
         <v>855</v>
       </c>
       <c r="K544" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="L544" t="s">
         <v>832</v>
@@ -19101,7 +19095,7 @@
         <v>856</v>
       </c>
       <c r="K545" t="s">
-        <v>960</v>
+        <v>934</v>
       </c>
       <c r="L545" t="s">
         <v>832</v>
@@ -19478,7 +19472,7 @@
         <v>855</v>
       </c>
       <c r="K558" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L558" t="s">
         <v>832</v>
@@ -19507,7 +19501,7 @@
         <v>856</v>
       </c>
       <c r="K559" t="s">
-        <v>961</v>
+        <v>935</v>
       </c>
       <c r="L559" t="s">
         <v>832</v>
@@ -19884,7 +19878,7 @@
         <v>855</v>
       </c>
       <c r="K572" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="L572" t="s">
         <v>832</v>
@@ -19913,7 +19907,7 @@
         <v>856</v>
       </c>
       <c r="K573" t="s">
-        <v>962</v>
+        <v>936</v>
       </c>
       <c r="L573" t="s">
         <v>832</v>
@@ -20290,7 +20284,7 @@
         <v>855</v>
       </c>
       <c r="K586" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="L586" t="s">
         <v>832</v>
@@ -20319,7 +20313,7 @@
         <v>856</v>
       </c>
       <c r="K587" t="s">
-        <v>963</v>
+        <v>937</v>
       </c>
       <c r="L587" t="s">
         <v>832</v>
@@ -20696,7 +20690,7 @@
         <v>855</v>
       </c>
       <c r="K600" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="L600" t="s">
         <v>832</v>
@@ -20725,7 +20719,7 @@
         <v>856</v>
       </c>
       <c r="K601" t="s">
-        <v>964</v>
+        <v>938</v>
       </c>
       <c r="L601" t="s">
         <v>832</v>
@@ -22181,7 +22175,7 @@
         <v>811</v>
       </c>
       <c r="M651" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.2">
@@ -23718,7 +23712,7 @@
         <v>811</v>
       </c>
       <c r="M704" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="705" spans="1:13" x14ac:dyDescent="0.2">
@@ -23747,7 +23741,7 @@
         <v>811</v>
       </c>
       <c r="M705" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="706" spans="1:13" x14ac:dyDescent="0.2">
@@ -23776,7 +23770,7 @@
         <v>811</v>
       </c>
       <c r="M706" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="707" spans="1:13" x14ac:dyDescent="0.2">
@@ -23834,7 +23828,7 @@
         <v>811</v>
       </c>
       <c r="M708" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="709" spans="1:13" x14ac:dyDescent="0.2">
@@ -24240,7 +24234,7 @@
         <v>811</v>
       </c>
       <c r="M722" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="723" spans="1:13" x14ac:dyDescent="0.2">
@@ -24269,7 +24263,7 @@
         <v>811</v>
       </c>
       <c r="M723" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row r="724" spans="1:13" x14ac:dyDescent="0.2">
@@ -25220,7 +25214,7 @@
         <v>866</v>
       </c>
       <c r="K756" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="L756" t="s">
         <v>832</v>
@@ -25249,7 +25243,7 @@
         <v>867</v>
       </c>
       <c r="K757" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="L757" t="s">
         <v>832</v>
@@ -25568,7 +25562,7 @@
         <v>871</v>
       </c>
       <c r="K768" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
       <c r="L768" t="s">
         <v>832</v>
@@ -25582,7 +25576,7 @@
         <v>768</v>
       </c>
       <c r="B769" t="s">
-        <v>967</v>
+        <v>941</v>
       </c>
       <c r="D769" t="s">
         <v>815</v>
@@ -25603,7 +25597,7 @@
         <v>811</v>
       </c>
       <c r="M769" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
     </row>
     <row r="770" spans="1:13" x14ac:dyDescent="0.2">
@@ -25632,7 +25626,7 @@
         <v>811</v>
       </c>
       <c r="M770" t="s">
-        <v>936</v>
+        <v>955</v>
       </c>
     </row>
     <row r="771" spans="1:13" x14ac:dyDescent="0.2">
@@ -25655,13 +25649,13 @@
         <v>872</v>
       </c>
       <c r="K771" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="L771" t="s">
         <v>832</v>
       </c>
       <c r="M771" t="s">
-        <v>937</v>
+        <v>956</v>
       </c>
     </row>
     <row r="772" spans="1:13" x14ac:dyDescent="0.2">
@@ -25681,16 +25675,16 @@
         <v>811</v>
       </c>
       <c r="I772" t="s">
-        <v>873</v>
+        <v>957</v>
       </c>
       <c r="K772" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="L772" t="s">
         <v>832</v>
       </c>
       <c r="M772" t="s">
-        <v>938</v>
+        <v>958</v>
       </c>
     </row>
     <row r="773" spans="1:13" x14ac:dyDescent="0.2">
@@ -25768,10 +25762,10 @@
         <v>811</v>
       </c>
       <c r="I775" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="K775" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="L775" t="s">
         <v>832</v>
@@ -25797,10 +25791,10 @@
         <v>811</v>
       </c>
       <c r="I776" t="s">
-        <v>875</v>
+        <v>959</v>
       </c>
       <c r="K776" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="L776" t="s">
         <v>832</v>
@@ -25971,7 +25965,7 @@
         <v>811</v>
       </c>
       <c r="I782" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="K782" t="s">
         <v>811</v>
@@ -26000,7 +25994,7 @@
         <v>811</v>
       </c>
       <c r="I783" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="K783" t="s">
         <v>811</v>
@@ -26029,10 +26023,10 @@
         <v>811</v>
       </c>
       <c r="I784" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="K784" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="L784" t="s">
         <v>832</v>
@@ -26058,10 +26052,10 @@
         <v>811</v>
       </c>
       <c r="I785" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="K785" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="L785" t="s">
         <v>832</v>
@@ -26162,7 +26156,7 @@
         <v>788</v>
       </c>
       <c r="B789" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="D789" t="s">
         <v>815</v>
@@ -26183,7 +26177,7 @@
         <v>811</v>
       </c>
       <c r="M789" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
     </row>
     <row r="790" spans="1:13" x14ac:dyDescent="0.2">
@@ -26191,7 +26185,7 @@
         <v>789</v>
       </c>
       <c r="B790" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="D790" t="s">
         <v>815</v>
@@ -26212,7 +26206,7 @@
         <v>811</v>
       </c>
       <c r="M790" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
     </row>
     <row r="791" spans="1:13" x14ac:dyDescent="0.2">
@@ -26220,7 +26214,7 @@
         <v>790</v>
       </c>
       <c r="B791" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="D791" t="s">
         <v>815</v>
@@ -26241,7 +26235,7 @@
         <v>811</v>
       </c>
       <c r="M791" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
     </row>
     <row r="792" spans="1:13" x14ac:dyDescent="0.2">
@@ -26249,7 +26243,7 @@
         <v>791</v>
       </c>
       <c r="B792" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="D792" t="s">
         <v>815</v>
@@ -26270,7 +26264,7 @@
         <v>811</v>
       </c>
       <c r="M792" t="s">
-        <v>956</v>
+        <v>963</v>
       </c>
     </row>
     <row r="793" spans="1:13" x14ac:dyDescent="0.2">
@@ -26278,7 +26272,7 @@
         <v>792</v>
       </c>
       <c r="B793" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="D793" t="s">
         <v>815</v>
@@ -26299,7 +26293,7 @@
         <v>811</v>
       </c>
       <c r="M793" t="s">
-        <v>957</v>
+        <v>964</v>
       </c>
     </row>
     <row r="794" spans="1:13" x14ac:dyDescent="0.2">
@@ -26307,7 +26301,7 @@
         <v>793</v>
       </c>
       <c r="B794" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="D794" t="s">
         <v>815</v>
@@ -26328,7 +26322,7 @@
         <v>811</v>
       </c>
       <c r="M794" t="s">
-        <v>958</v>
+        <v>965</v>
       </c>
     </row>
     <row r="795" spans="1:13" x14ac:dyDescent="0.2">
@@ -26348,7 +26342,7 @@
         <v>832</v>
       </c>
       <c r="I795" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="K795" t="s">
         <v>811</v>
@@ -26676,7 +26670,7 @@
         <v>811</v>
       </c>
       <c r="M806" t="s">
-        <v>939</v>
+        <v>966</v>
       </c>
     </row>
     <row r="807" spans="1:13" x14ac:dyDescent="0.2">
@@ -26705,7 +26699,7 @@
         <v>811</v>
       </c>
       <c r="M807" t="s">
-        <v>940</v>
+        <v>967</v>
       </c>
     </row>
     <row r="808" spans="1:13" x14ac:dyDescent="0.2">
@@ -26734,7 +26728,7 @@
         <v>811</v>
       </c>
       <c r="M808" t="s">
-        <v>941</v>
+        <v>968</v>
       </c>
     </row>
     <row r="809" spans="1:13" x14ac:dyDescent="0.2">
@@ -26742,7 +26736,7 @@
         <v>808</v>
       </c>
       <c r="B809" t="s">
-        <v>966</v>
+        <v>940</v>
       </c>
       <c r="D809" t="s">
         <v>817</v>
@@ -26771,7 +26765,7 @@
         <v>809</v>
       </c>
       <c r="B810" t="s">
-        <v>966</v>
+        <v>940</v>
       </c>
       <c r="D810" t="s">
         <v>817</v>
@@ -26800,7 +26794,7 @@
         <v>810</v>
       </c>
       <c r="B811" t="s">
-        <v>966</v>
+        <v>940</v>
       </c>
       <c r="D811" t="s">
         <v>817</v>

</xml_diff>

<commit_message>
gra2005 + gra2009 new storageType
</commit_message>
<xml_diff>
--- a/data/variables/ds1/variables.xlsx
+++ b/data/variables/ds1/variables.xlsx
@@ -8562,8 +8562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1897" workbookViewId="0">
-      <selection activeCell="C1916" sqref="C1916"/>
+    <sheetView tabSelected="1" topLeftCell="A1478" workbookViewId="0">
+      <selection activeCell="B1502" sqref="B1502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8738,7 +8738,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C5" t="s">
         <v>2219</v>
@@ -8814,7 +8814,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C7" t="s">
         <v>2219</v>
@@ -9574,7 +9574,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C27" t="s">
         <v>2219</v>
@@ -9650,7 +9650,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C29" t="s">
         <v>2219</v>
@@ -10410,7 +10410,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C49" t="s">
         <v>2219</v>
@@ -10486,7 +10486,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C51" t="s">
         <v>2219</v>
@@ -11246,7 +11246,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C71" t="s">
         <v>2219</v>
@@ -11322,7 +11322,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C73" t="s">
         <v>2219</v>
@@ -12082,7 +12082,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C93" t="s">
         <v>2219</v>
@@ -12158,7 +12158,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C95" t="s">
         <v>2219</v>
@@ -12918,7 +12918,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C115" t="s">
         <v>2219</v>
@@ -13602,7 +13602,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C133" t="s">
         <v>2219</v>
@@ -14286,7 +14286,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C151" t="s">
         <v>2219</v>
@@ -15046,7 +15046,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C171" t="s">
         <v>2219</v>
@@ -20936,7 +20936,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C326" t="s">
         <v>2219</v>
@@ -21050,7 +21050,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C329" t="s">
         <v>2219</v>
@@ -22266,7 +22266,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C361" t="s">
         <v>2219</v>
@@ -22380,7 +22380,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C364" t="s">
         <v>2219</v>
@@ -28384,7 +28384,7 @@
         <v>521</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C522" t="s">
         <v>2268</v>
@@ -28460,7 +28460,7 @@
         <v>523</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C524" t="s">
         <v>2270</v>
@@ -28916,7 +28916,7 @@
         <v>535</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C536" t="s">
         <v>2282</v>
@@ -28992,7 +28992,7 @@
         <v>537</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C538" t="s">
         <v>2284</v>
@@ -29448,7 +29448,7 @@
         <v>549</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C550" t="s">
         <v>2296</v>
@@ -29524,7 +29524,7 @@
         <v>551</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C552" t="s">
         <v>2298</v>
@@ -29980,7 +29980,7 @@
         <v>563</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C564" t="s">
         <v>2310</v>
@@ -30056,7 +30056,7 @@
         <v>565</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C566" t="s">
         <v>2312</v>
@@ -30512,7 +30512,7 @@
         <v>577</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C578" t="s">
         <v>2324</v>
@@ -30588,7 +30588,7 @@
         <v>579</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C580" t="s">
         <v>2326</v>
@@ -31044,7 +31044,7 @@
         <v>591</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C592" t="s">
         <v>2338</v>
@@ -31120,7 +31120,7 @@
         <v>593</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C594" t="s">
         <v>2340</v>
@@ -37200,7 +37200,7 @@
         <v>753</v>
       </c>
       <c r="B754" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C754" t="s">
         <v>2219</v>
@@ -37580,7 +37580,7 @@
         <v>763</v>
       </c>
       <c r="B764" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C764" t="s">
         <v>2219</v>
@@ -37732,7 +37732,7 @@
         <v>767</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C768" t="s">
         <v>2219</v>
@@ -37770,7 +37770,7 @@
         <v>768</v>
       </c>
       <c r="B769" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C769" t="s">
         <v>2219</v>
@@ -38112,7 +38112,7 @@
         <v>777</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C778" t="s">
         <v>2219</v>
@@ -38606,7 +38606,7 @@
         <v>790</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C791" t="s">
         <v>2424</v>
@@ -38682,7 +38682,7 @@
         <v>792</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C793" t="s">
         <v>2426</v>
@@ -38758,7 +38758,7 @@
         <v>794</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C795" t="s">
         <v>2428</v>
@@ -39290,7 +39290,7 @@
         <v>808</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C809" t="s">
         <v>2431</v>
@@ -41152,7 +41152,7 @@
         <v>857</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C858" t="s">
         <v>2219</v>
@@ -41228,7 +41228,7 @@
         <v>859</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C860" t="s">
         <v>2219</v>
@@ -44382,7 +44382,7 @@
         <v>942</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C943" t="s">
         <v>2268</v>
@@ -44458,7 +44458,7 @@
         <v>944</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C945" t="s">
         <v>2270</v>
@@ -44952,7 +44952,7 @@
         <v>957</v>
       </c>
       <c r="B958" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C958" t="s">
         <v>2282</v>
@@ -45028,7 +45028,7 @@
         <v>959</v>
       </c>
       <c r="B960" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C960" t="s">
         <v>2284</v>
@@ -45522,7 +45522,7 @@
         <v>972</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C973" t="s">
         <v>2296</v>
@@ -45598,7 +45598,7 @@
         <v>974</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C975" t="s">
         <v>2298</v>
@@ -46092,7 +46092,7 @@
         <v>987</v>
       </c>
       <c r="B988" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C988" t="s">
         <v>2310</v>
@@ -46168,7 +46168,7 @@
         <v>989</v>
       </c>
       <c r="B990" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C990" t="s">
         <v>2312</v>
@@ -46662,7 +46662,7 @@
         <v>1002</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1003" t="s">
         <v>2324</v>
@@ -46738,7 +46738,7 @@
         <v>1004</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1005" t="s">
         <v>2326</v>
@@ -47232,7 +47232,7 @@
         <v>1017</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1018" t="s">
         <v>2338</v>
@@ -47308,7 +47308,7 @@
         <v>1019</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1020" t="s">
         <v>2340</v>
@@ -47802,7 +47802,7 @@
         <v>1032</v>
       </c>
       <c r="B1033" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1033" t="s">
         <v>2219</v>
@@ -47878,7 +47878,7 @@
         <v>1034</v>
       </c>
       <c r="B1035" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1035" t="s">
         <v>2219</v>
@@ -48372,7 +48372,7 @@
         <v>1047</v>
       </c>
       <c r="B1048" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1048" t="s">
         <v>2219</v>
@@ -53578,7 +53578,7 @@
         <v>1184</v>
       </c>
       <c r="B1185" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1185" t="s">
         <v>2219</v>
@@ -54224,7 +54224,7 @@
         <v>1201</v>
       </c>
       <c r="B1202" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1202" t="s">
         <v>2219</v>
@@ -54300,7 +54300,7 @@
         <v>1203</v>
       </c>
       <c r="B1204" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1204" t="s">
         <v>2219</v>
@@ -54946,7 +54946,7 @@
         <v>1220</v>
       </c>
       <c r="B1221" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1221" t="s">
         <v>2219</v>
@@ -55022,7 +55022,7 @@
         <v>1222</v>
       </c>
       <c r="B1223" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1223" t="s">
         <v>2219</v>
@@ -55668,7 +55668,7 @@
         <v>1239</v>
       </c>
       <c r="B1240" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1240" t="s">
         <v>2219</v>
@@ -55744,7 +55744,7 @@
         <v>1241</v>
       </c>
       <c r="B1242" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1242" t="s">
         <v>2219</v>
@@ -56390,7 +56390,7 @@
         <v>1258</v>
       </c>
       <c r="B1259" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1259" t="s">
         <v>2219</v>
@@ -56466,7 +56466,7 @@
         <v>1260</v>
       </c>
       <c r="B1261" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1261" t="s">
         <v>2219</v>
@@ -65586,7 +65586,7 @@
         <v>1500</v>
       </c>
       <c r="B1501" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1501" t="s">
         <v>2431</v>
@@ -69576,7 +69576,7 @@
         <v>1605</v>
       </c>
       <c r="B1606" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1606" t="s">
         <v>2219</v>
@@ -69652,7 +69652,7 @@
         <v>1607</v>
       </c>
       <c r="B1608" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1608" t="s">
         <v>2219</v>
@@ -70944,7 +70944,7 @@
         <v>1641</v>
       </c>
       <c r="B1642" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1642" t="s">
         <v>2219</v>
@@ -71020,7 +71020,7 @@
         <v>1643</v>
       </c>
       <c r="B1644" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1644" t="s">
         <v>2219</v>
@@ -72312,7 +72312,7 @@
         <v>1677</v>
       </c>
       <c r="B1678" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1678" t="s">
         <v>2219</v>
@@ -72388,7 +72388,7 @@
         <v>1679</v>
       </c>
       <c r="B1680" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1680" t="s">
         <v>2219</v>
@@ -75048,7 +75048,7 @@
         <v>1749</v>
       </c>
       <c r="B1750" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1750" t="s">
         <v>2219</v>
@@ -75124,7 +75124,7 @@
         <v>1751</v>
       </c>
       <c r="B1752" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1752" t="s">
         <v>2219</v>
@@ -76416,7 +76416,7 @@
         <v>1785</v>
       </c>
       <c r="B1786" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1786" t="s">
         <v>2219</v>
@@ -76492,7 +76492,7 @@
         <v>1787</v>
       </c>
       <c r="B1788" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C1788" t="s">
         <v>2219</v>
@@ -84662,7 +84662,7 @@
         <v>2002</v>
       </c>
       <c r="B2003" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C2003" t="s">
         <v>2219</v>
@@ -84738,7 +84738,7 @@
         <v>2004</v>
       </c>
       <c r="B2005" s="1" t="s">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="C2005" t="s">
         <v>2219</v>
@@ -84966,7 +84966,7 @@
         <v>2010</v>
       </c>
       <c r="B2011" s="1" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="C2011" t="s">
         <v>2219</v>

</xml_diff>